<commit_message>
[Task 10] v3 Render markers and polylines in leaflet map.
	- Draw markers for current location and destination.
	- Draw all polylines based on the possible paths generate by dfs recursive function.
</commit_message>
<xml_diff>
--- a/edges.xlsx
+++ b/edges.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="6120"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="edges sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -387,7 +387,7 @@
   <dimension ref="A1:C99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C108" sqref="B108:C108"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>